<commit_message>
Use Leaderboard_Template.xlsx is current tournament has no existing file
	-- Open Leaderboard_Template.xlsx, update data and save as:
	-- '{} -- {}.xlsx'.format(tname, tyear)
</commit_message>
<xml_diff>
--- a/Leaderboard_Template.xlsx
+++ b/Leaderboard_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="45210" yWindow="3690" windowWidth="25845" windowHeight="17190"/>
+    <workbookView xWindow="45210" yWindow="3690" windowWidth="25845" windowHeight="17190" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -1818,7 +1818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -11345,7 +11345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add Live Tab to Leaderboard_Template.xlsx and make it default sheet
</commit_message>
<xml_diff>
--- a/Leaderboard_Template.xlsx
+++ b/Leaderboard_Template.xlsx
@@ -12,10 +12,11 @@
     <workbookView xWindow="45210" yWindow="3690" windowWidth="25845" windowHeight="17190"/>
   </bookViews>
   <sheets>
-    <sheet name="Results" sheetId="1" r:id="rId1"/>
-    <sheet name="Clean Data" sheetId="2" r:id="rId2"/>
-    <sheet name="Raw Data" sheetId="3" r:id="rId3"/>
-    <sheet name="Details" sheetId="4" r:id="rId4"/>
+    <sheet name="Live" sheetId="5" r:id="rId1"/>
+    <sheet name="Results" sheetId="1" r:id="rId2"/>
+    <sheet name="Clean Data" sheetId="2" r:id="rId3"/>
+    <sheet name="Raw Data" sheetId="3" r:id="rId4"/>
+    <sheet name="Details" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="course_id">Details!$B$9</definedName>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="452">
   <si>
     <t>Thursday Total</t>
   </si>
@@ -1816,10 +1817,685 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="3" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="6" t="str">
+        <f>tname&amp;" -- "&amp;YEAR(start_date)</f>
+        <v>Valero Texas Open -- 2019</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2">
+        <v>6</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="5">
+        <f>SUM(VLOOKUP($B4,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C4,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D4,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E4,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F4,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G4,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-431</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="5">
+        <f>SUM(VLOOKUP($B5,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C5,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D5,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E5,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F5,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G5,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-411</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="5">
+        <f>SUM(VLOOKUP($B6,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C6,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D6,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E6,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F6,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G6,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="5">
+        <f>SUM(VLOOKUP($B7,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C7,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D7,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E7,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F7,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G7,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-438</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="5">
+        <f>SUM(VLOOKUP($B8,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C8,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D8,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E8,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F8,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G8,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-446</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="5">
+        <f>SUM(VLOOKUP($B9,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C9,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D9,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E9,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F9,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G9,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-370</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="5">
+        <f>SUM(VLOOKUP($B10,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C10,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D10,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E10,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F10,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G10,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-434</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="5">
+        <f>SUM(VLOOKUP($B11,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C11,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D11,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E11,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F11,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G11,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-471</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="5">
+        <f>SUM(VLOOKUP($B12,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C12,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D12,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E12,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F12,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G12,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-483</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="5">
+        <f>SUM(VLOOKUP($B13,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C13,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D13,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E13,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F13,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G13,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-416</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="5">
+        <f>SUM(VLOOKUP($B14,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C14,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D14,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E14,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F14,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G14,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-447</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="5">
+        <f>SUM(VLOOKUP($B15,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C15,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D15,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E15,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F15,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G15,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-393</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="5">
+        <f>SUM(VLOOKUP($B16,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C16,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D16,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E16,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F16,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G16,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-406</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="5">
+        <f>SUM(VLOOKUP($B17,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C17,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D17,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E17,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F17,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G17,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-360</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="5">
+        <f>SUM(VLOOKUP($B18,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C18,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D18,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E18,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F18,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G18,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-406</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="5">
+        <f>SUM(VLOOKUP($B19,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C19,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D19,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E19,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F19,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G19,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-387</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="5">
+        <f>SUM(VLOOKUP($B20,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C20,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D20,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E20,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F20,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G20,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-367</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="5">
+        <f>SUM(VLOOKUP($B21,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C21,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D21,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E21,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F21,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G21,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-391</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="5">
+        <f>SUM(VLOOKUP($B22,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C22,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D22,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E22,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F22,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G22,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-432</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="5">
+        <f>SUM(VLOOKUP($B23,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C23,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D23,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E23,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F23,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G23,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+        <v>-377</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2851,7 +3527,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M157"/>
   <sheetViews>
@@ -11341,7 +12017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R145"/>
   <sheetViews>
@@ -17957,7 +18633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fix Masters Picks.csv and fixed code to use it
</commit_message>
<xml_diff>
--- a/Leaderboard_Template.xlsx
+++ b/Leaderboard_Template.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Programming\golf_pool\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77F39DF-BFC1-4DF8-AD12-5EFEFFBAA9AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="3780" windowWidth="25845" windowHeight="17190"/>
+    <workbookView xWindow="47025" yWindow="5505" windowWidth="27165" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Live" sheetId="5" r:id="rId1"/>
     <sheet name="Results" sheetId="1" r:id="rId2"/>
-    <sheet name="Clean Data" sheetId="2" r:id="rId3"/>
+    <sheet name="Clean Data" sheetId="2" state="hidden" r:id="rId3"/>
     <sheet name="Raw Data" sheetId="3" r:id="rId4"/>
     <sheet name="Details" sheetId="4" r:id="rId5"/>
   </sheets>
@@ -38,7 +39,7 @@
     <definedName name="tid">Details!$B$1</definedName>
     <definedName name="tname">Details!$B$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -374,20 +375,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\+#0_);[Red]\-#0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -456,24 +449,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -778,11 +768,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +783,7 @@
     <col min="9" max="9" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -807,18 +797,18 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="6" t="str">
+      <c r="A2" s="5" t="str">
         <f>tname&amp;" -- "&amp;YEAR(start_date)</f>
         <v>Valero Texas Open -- 2019</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -849,272 +839,272 @@
       <c r="A4" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>64</v>
       </c>
       <c r="H4" s="3"/>
-      <c r="I4" s="5">
-        <f>SUM(VLOOKUP($B4,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C4,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D4,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E4,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F4,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G4,'Clean Data'!$A$2:$M$157,I$1,0))</f>
-        <v>-271</v>
+      <c r="I4" s="4">
+        <f>SUM(VLOOKUP($B4,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($C4,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($D4,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($E4,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($F4,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($G4,'Raw Data'!$B$2:$R$157,I$1,0))</f>
+        <v>-55</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>71</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="5">
-        <f>SUM(VLOOKUP($B5,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C5,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D5,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E5,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F5,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G5,'Clean Data'!$A$2:$M$157,I$1,0))</f>
-        <v>-648</v>
+      <c r="I5" s="4">
+        <f>SUM(VLOOKUP($B5,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($C5,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($D5,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($E5,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($F5,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($G5,'Raw Data'!$B$2:$R$157,I$1,0))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="5">
-        <f>SUM(VLOOKUP($B6,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C6,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D6,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E6,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F6,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G6,'Clean Data'!$A$2:$M$157,I$1,0))</f>
-        <v>-1059</v>
+      <c r="I6" s="4">
+        <f>SUM(VLOOKUP($B6,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($C6,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($D6,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($E6,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($F6,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($G6,'Raw Data'!$B$2:$R$157,I$1,0))</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="5"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="5"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="5"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="5"/>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="5"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="5"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="1"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="5"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="1"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="5"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="1"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="5"/>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="5"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="5"/>
+      <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="5"/>
+      <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="5"/>
+      <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="5"/>
+      <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="4"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="5"/>
+      <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="5"/>
+      <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="1"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="5"/>
+      <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
@@ -1125,7 +1115,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -1136,7 +1126,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -1147,12 +1137,854 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
+      <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="4"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="4"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="4"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="4"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="4"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="4"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="4"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="4"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="4"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="4"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="4"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="4"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="4"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="4"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="4"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="4"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="4"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="4"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="4"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="4"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="4"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="4"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="4"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="4"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="4"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="4"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="4"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="4"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="4"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="4"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="4"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="4"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="4"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="4"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="3"/>
+      <c r="I84" s="4"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="4"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="3"/>
+      <c r="I86" s="4"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+      <c r="I87" s="4"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="4"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="4"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="4"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="4"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
+      <c r="I92" s="4"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3"/>
+      <c r="I93" s="4"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="3"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="3"/>
+      <c r="I94" s="4"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="3"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
+      <c r="I95" s="4"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="3"/>
+      <c r="I96" s="4"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="3"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3"/>
+      <c r="I97" s="4"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
+      <c r="H98" s="3"/>
+      <c r="I98" s="4"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3"/>
+      <c r="I99" s="4"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="3"/>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
+      <c r="H100" s="3"/>
+      <c r="I100" s="4"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="3"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+      <c r="I101" s="4"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="3"/>
+      <c r="B102" s="3"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
+      <c r="I102" s="4"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="3"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+      <c r="I103" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1164,11 +1996,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M103"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,22 +2035,22 @@
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="6" t="str">
+      <c r="A2" s="5" t="str">
         <f>tname&amp;" -- "&amp;YEAR(start_date)</f>
         <v>Valero Texas Open -- 2019</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -1261,42 +2093,42 @@
       <c r="A4" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>64</v>
       </c>
       <c r="H4" s="3"/>
-      <c r="I4" s="5">
-        <f>SUM(VLOOKUP($B4,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C4,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D4,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E4,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F4,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G4,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+      <c r="I4" s="4">
+        <f>SUM(VLOOKUP($B4,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($C4,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($D4,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($E4,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($F4,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($G4,'Raw Data'!$B$2:$R$157,I$1,0))-(par_total*6)</f>
         <v>-13</v>
       </c>
-      <c r="J4" s="5">
-        <f>SUM(VLOOKUP($B4,'Clean Data'!$A$2:$M$157,J$1,0),VLOOKUP($C4,'Clean Data'!$A$2:$M$157,J$1,0),VLOOKUP($D4,'Clean Data'!$A$2:$M$157,J$1,0),VLOOKUP($E4,'Clean Data'!$A$2:$M$157,J$1,0),VLOOKUP($F4,'Clean Data'!$A$2:$M$157,J$1,0),VLOOKUP($G4,'Clean Data'!$A$2:$M$157,J$1,0))-(par_total*6)</f>
+      <c r="J4" s="4">
+        <f>SUM(VLOOKUP($B4,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($C4,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($D4,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($E4,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($F4,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($G4,'Raw Data'!$B$2:$R$157,J$1,0))-(par_total*6)</f>
         <v>-12</v>
       </c>
-      <c r="K4" s="5">
-        <f>SUM(VLOOKUP($B4,'Clean Data'!$A$2:$M$157,K$1,0),VLOOKUP($C4,'Clean Data'!$A$2:$M$157,K$1,0),VLOOKUP($D4,'Clean Data'!$A$2:$M$157,K$1,0),VLOOKUP($E4,'Clean Data'!$A$2:$M$157,K$1,0),VLOOKUP($F4,'Clean Data'!$A$2:$M$157,K$1,0),VLOOKUP($G4,'Clean Data'!$A$2:$M$157,K$1,0))-(par_total*6)</f>
+      <c r="K4" s="4">
+        <f>SUM(VLOOKUP($B4,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($C4,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($D4,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($E4,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($F4,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($G4,'Raw Data'!$B$2:$R$157,K$1,0))-(par_total*6)</f>
         <v>-11</v>
       </c>
-      <c r="L4" s="5">
-        <f>SUM(VLOOKUP($B4,'Clean Data'!$A$2:$M$157,L$1,0),VLOOKUP($C4,'Clean Data'!$A$2:$M$157,L$1,0),VLOOKUP($D4,'Clean Data'!$A$2:$M$157,L$1,0),VLOOKUP($E4,'Clean Data'!$A$2:$M$157,L$1,0),VLOOKUP($F4,'Clean Data'!$A$2:$M$157,L$1,0),VLOOKUP($G4,'Clean Data'!$A$2:$M$157,L$1,0))-(par_total*6)</f>
+      <c r="L4" s="4">
+        <f>SUM(VLOOKUP($B4,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($C4,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($D4,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($E4,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($F4,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($G4,'Raw Data'!$B$2:$R$157,L$1,0))-(par_total*6)</f>
         <v>-235</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <f t="shared" ref="M4:M6" si="0">+SUM(I4:L4)</f>
         <v>-271</v>
       </c>
@@ -1305,42 +2137,42 @@
       <c r="A5" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>71</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="5">
-        <f>SUM(VLOOKUP($B5,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C5,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D5,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E5,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F5,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G5,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="5">
-        <f>SUM(VLOOKUP($B5,'Clean Data'!$A$2:$M$157,J$1,0),VLOOKUP($C5,'Clean Data'!$A$2:$M$157,J$1,0),VLOOKUP($D5,'Clean Data'!$A$2:$M$157,J$1,0),VLOOKUP($E5,'Clean Data'!$A$2:$M$157,J$1,0),VLOOKUP($F5,'Clean Data'!$A$2:$M$157,J$1,0),VLOOKUP($G5,'Clean Data'!$A$2:$M$157,J$1,0))-(par_total*6)</f>
+      <c r="I5" s="4">
+        <f>SUM(VLOOKUP($B5,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($C5,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($D5,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($E5,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($F5,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($G5,'Raw Data'!$B$2:$R$157,I$1,0))-(par_total*6)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <f>SUM(VLOOKUP($B5,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($C5,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($D5,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($E5,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($F5,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($G5,'Raw Data'!$B$2:$R$157,J$1,0))-(par_total*6)</f>
         <v>-6</v>
       </c>
-      <c r="K5" s="5">
-        <f>SUM(VLOOKUP($B5,'Clean Data'!$A$2:$M$157,K$1,0),VLOOKUP($C5,'Clean Data'!$A$2:$M$157,K$1,0),VLOOKUP($D5,'Clean Data'!$A$2:$M$157,K$1,0),VLOOKUP($E5,'Clean Data'!$A$2:$M$157,K$1,0),VLOOKUP($F5,'Clean Data'!$A$2:$M$157,K$1,0),VLOOKUP($G5,'Clean Data'!$A$2:$M$157,K$1,0))-(par_total*6)</f>
+      <c r="K5" s="4">
+        <f>SUM(VLOOKUP($B5,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($C5,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($D5,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($E5,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($F5,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($G5,'Raw Data'!$B$2:$R$157,K$1,0))-(par_total*6)</f>
         <v>-210</v>
       </c>
-      <c r="L5" s="5">
-        <f>SUM(VLOOKUP($B5,'Clean Data'!$A$2:$M$157,L$1,0),VLOOKUP($C5,'Clean Data'!$A$2:$M$157,L$1,0),VLOOKUP($D5,'Clean Data'!$A$2:$M$157,L$1,0),VLOOKUP($E5,'Clean Data'!$A$2:$M$157,L$1,0),VLOOKUP($F5,'Clean Data'!$A$2:$M$157,L$1,0),VLOOKUP($G5,'Clean Data'!$A$2:$M$157,L$1,0))-(par_total*6)</f>
+      <c r="L5" s="4">
+        <f>SUM(VLOOKUP($B5,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($C5,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($D5,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($E5,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($F5,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($G5,'Raw Data'!$B$2:$R$157,L$1,0))-(par_total*6)</f>
         <v>-432</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="4">
         <f t="shared" si="0"/>
         <v>-648</v>
       </c>
@@ -1349,300 +2181,300 @@
       <c r="A6" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="5">
-        <f>SUM(VLOOKUP($B6,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($C6,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($D6,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($E6,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($F6,'Clean Data'!$A$2:$M$157,I$1,0),VLOOKUP($G6,'Clean Data'!$A$2:$M$157,I$1,0))-(par_total*6)</f>
+      <c r="I6" s="4">
+        <f>SUM(VLOOKUP($B6,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($C6,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($D6,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($E6,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($F6,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($G6,'Raw Data'!$B$2:$R$157,I$1,0))-(par_total*6)</f>
         <v>-28</v>
       </c>
-      <c r="J6" s="5">
-        <f>SUM(VLOOKUP($B6,'Clean Data'!$A$2:$M$157,J$1,0),VLOOKUP($C6,'Clean Data'!$A$2:$M$157,J$1,0),VLOOKUP($D6,'Clean Data'!$A$2:$M$157,J$1,0),VLOOKUP($E6,'Clean Data'!$A$2:$M$157,J$1,0),VLOOKUP($F6,'Clean Data'!$A$2:$M$157,J$1,0),VLOOKUP($G6,'Clean Data'!$A$2:$M$157,J$1,0))-(par_total*6)</f>
+      <c r="J6" s="4">
+        <f>SUM(VLOOKUP($B6,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($C6,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($D6,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($E6,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($F6,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($G6,'Raw Data'!$B$2:$R$157,J$1,0))-(par_total*6)</f>
         <v>-167</v>
       </c>
-      <c r="K6" s="5">
-        <f>SUM(VLOOKUP($B6,'Clean Data'!$A$2:$M$157,K$1,0),VLOOKUP($C6,'Clean Data'!$A$2:$M$157,K$1,0),VLOOKUP($D6,'Clean Data'!$A$2:$M$157,K$1,0),VLOOKUP($E6,'Clean Data'!$A$2:$M$157,K$1,0),VLOOKUP($F6,'Clean Data'!$A$2:$M$157,K$1,0),VLOOKUP($G6,'Clean Data'!$A$2:$M$157,K$1,0))-(par_total*6)</f>
+      <c r="K6" s="4">
+        <f>SUM(VLOOKUP($B6,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($C6,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($D6,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($E6,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($F6,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($G6,'Raw Data'!$B$2:$R$157,K$1,0))-(par_total*6)</f>
         <v>-432</v>
       </c>
-      <c r="L6" s="5">
-        <f>SUM(VLOOKUP($B6,'Clean Data'!$A$2:$M$157,L$1,0),VLOOKUP($C6,'Clean Data'!$A$2:$M$157,L$1,0),VLOOKUP($D6,'Clean Data'!$A$2:$M$157,L$1,0),VLOOKUP($E6,'Clean Data'!$A$2:$M$157,L$1,0),VLOOKUP($F6,'Clean Data'!$A$2:$M$157,L$1,0),VLOOKUP($G6,'Clean Data'!$A$2:$M$157,L$1,0))-(par_total*6)</f>
+      <c r="L6" s="4">
+        <f>SUM(VLOOKUP($B6,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($C6,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($D6,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($E6,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($F6,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($G6,'Raw Data'!$B$2:$R$157,L$1,0))-(par_total*6)</f>
         <v>-432</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="4">
         <f t="shared" si="0"/>
         <v>-1059</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="1"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="1"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="1"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="4"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="1"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
@@ -1653,11 +2485,11 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -1668,11 +2500,11 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -1683,20 +2515,1166 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="4"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="4"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="4"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="4"/>
+      <c r="L63" s="4"/>
+      <c r="M63" s="4"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="4"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="4"/>
+      <c r="L65" s="4"/>
+      <c r="M65" s="4"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="4"/>
+      <c r="M66" s="4"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="4"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4"/>
+      <c r="M68" s="4"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="4"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="4"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
+      <c r="M71" s="4"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="4"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
+      <c r="M73" s="4"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="4"/>
+      <c r="L74" s="4"/>
+      <c r="M74" s="4"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="4"/>
+      <c r="K75" s="4"/>
+      <c r="L75" s="4"/>
+      <c r="M75" s="4"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="4"/>
+      <c r="K76" s="4"/>
+      <c r="L76" s="4"/>
+      <c r="M76" s="4"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="4"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="4"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="4"/>
+      <c r="K78" s="4"/>
+      <c r="L78" s="4"/>
+      <c r="M78" s="4"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="4"/>
+      <c r="K79" s="4"/>
+      <c r="L79" s="4"/>
+      <c r="M79" s="4"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="4"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="4"/>
+      <c r="J81" s="4"/>
+      <c r="K81" s="4"/>
+      <c r="L81" s="4"/>
+      <c r="M81" s="4"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="4"/>
+      <c r="K82" s="4"/>
+      <c r="L82" s="4"/>
+      <c r="M82" s="4"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="4"/>
+      <c r="J83" s="4"/>
+      <c r="K83" s="4"/>
+      <c r="L83" s="4"/>
+      <c r="M83" s="4"/>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="3"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="4"/>
+      <c r="L84" s="4"/>
+      <c r="M84" s="4"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="4"/>
+      <c r="J85" s="4"/>
+      <c r="K85" s="4"/>
+      <c r="L85" s="4"/>
+      <c r="M85" s="4"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="3"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
+      <c r="L86" s="4"/>
+      <c r="M86" s="4"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+      <c r="I87" s="4"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="4"/>
+      <c r="L87" s="4"/>
+      <c r="M87" s="4"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
+      <c r="L88" s="4"/>
+      <c r="M88" s="4"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
+      <c r="L89" s="4"/>
+      <c r="M89" s="4"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
+      <c r="L90" s="4"/>
+      <c r="M90" s="4"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="4"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="4"/>
+      <c r="L91" s="4"/>
+      <c r="M91" s="4"/>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
+      <c r="I92" s="4"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="4"/>
+      <c r="L92" s="4"/>
+      <c r="M92" s="4"/>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3"/>
+      <c r="I93" s="4"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="4"/>
+      <c r="L93" s="4"/>
+      <c r="M93" s="4"/>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94" s="3"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="3"/>
+      <c r="I94" s="4"/>
+      <c r="J94" s="4"/>
+      <c r="K94" s="4"/>
+      <c r="L94" s="4"/>
+      <c r="M94" s="4"/>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95" s="3"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
+      <c r="I95" s="4"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="4"/>
+      <c r="L95" s="4"/>
+      <c r="M95" s="4"/>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="3"/>
+      <c r="I96" s="4"/>
+      <c r="J96" s="4"/>
+      <c r="K96" s="4"/>
+      <c r="L96" s="4"/>
+      <c r="M96" s="4"/>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A97" s="3"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3"/>
+      <c r="I97" s="4"/>
+      <c r="J97" s="4"/>
+      <c r="K97" s="4"/>
+      <c r="L97" s="4"/>
+      <c r="M97" s="4"/>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
+      <c r="H98" s="3"/>
+      <c r="I98" s="4"/>
+      <c r="J98" s="4"/>
+      <c r="K98" s="4"/>
+      <c r="L98" s="4"/>
+      <c r="M98" s="4"/>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3"/>
+      <c r="I99" s="4"/>
+      <c r="J99" s="4"/>
+      <c r="K99" s="4"/>
+      <c r="L99" s="4"/>
+      <c r="M99" s="4"/>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A100" s="3"/>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
+      <c r="H100" s="3"/>
+      <c r="I100" s="4"/>
+      <c r="J100" s="4"/>
+      <c r="K100" s="4"/>
+      <c r="L100" s="4"/>
+      <c r="M100" s="4"/>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A101" s="3"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+      <c r="I101" s="4"/>
+      <c r="J101" s="4"/>
+      <c r="K101" s="4"/>
+      <c r="L101" s="4"/>
+      <c r="M101" s="4"/>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A102" s="3"/>
+      <c r="B102" s="3"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
+      <c r="I102" s="4"/>
+      <c r="J102" s="4"/>
+      <c r="K102" s="4"/>
+      <c r="L102" s="4"/>
+      <c r="M102" s="4"/>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103" s="3"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+      <c r="I103" s="4"/>
+      <c r="J103" s="4"/>
+      <c r="K103" s="4"/>
+      <c r="L103" s="4"/>
+      <c r="M103" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1708,11 +3686,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10198,11 +12176,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10709,13 +12687,14 @@
         <v>57</v>
       </c>
     </row>
+    <row r="22" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Update Template.xlsx and Add update time to Live sheet
</commit_message>
<xml_diff>
--- a/Leaderboard_Template.xlsx
+++ b/Leaderboard_Template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Programming\golf_pool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77F39DF-BFC1-4DF8-AD12-5EFEFFBAA9AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47025" yWindow="5505" windowWidth="27165" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47025" yWindow="5505" windowWidth="27165" windowHeight="14565"/>
   </bookViews>
   <sheets>
     <sheet name="Live" sheetId="5" r:id="rId1"/>
@@ -38,8 +37,9 @@
     <definedName name="start_date">Details!$B$3</definedName>
     <definedName name="tid">Details!$B$1</definedName>
     <definedName name="tname">Details!$B$2</definedName>
+    <definedName name="update_time">Details!$B$17</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="108">
   <si>
     <t>Thursday Total</t>
   </si>
@@ -371,15 +371,22 @@
   <si>
     <t>Best</t>
   </si>
+  <si>
+    <t>update_time</t>
+  </si>
+  <si>
+    <t>As of:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="\+#0_);[Red]\-#0"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,6 +406,13 @@
       <b/>
       <u/>
       <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -449,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -467,6 +481,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,11 +786,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I103"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:A24"/>
+      <selection activeCell="A2" sqref="A2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,7 +801,7 @@
     <col min="9" max="9" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -796,7 +814,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="str">
         <f>tname&amp;" -- "&amp;YEAR(start_date)</f>
         <v>Valero Texas Open -- 2019</v>
@@ -809,8 +827,11 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2">
         <v>1</v>
@@ -834,8 +855,12 @@
       <c r="I3" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="7">
+        <f>update_time</f>
+        <v>43567.381585648152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>105</v>
       </c>
@@ -863,7 +888,7 @@
         <v>-55</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>104</v>
       </c>
@@ -891,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>103</v>
       </c>
@@ -919,7 +944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -930,7 +955,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -941,7 +966,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -952,7 +977,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -963,7 +988,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -974,7 +999,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -985,7 +1010,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -996,7 +1021,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1007,7 +1032,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1018,7 +1043,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1996,11 +2021,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M103"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2021,16 +2046,20 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1">
+        <f>IF(current_round=1,5,6)</f>
         <v>6</v>
       </c>
       <c r="J1" s="1">
+        <f>IF(current_round=2,5,7)</f>
         <v>7</v>
       </c>
       <c r="K1" s="1">
+        <f>IF(current_round=3,5,8)</f>
         <v>8</v>
       </c>
       <c r="L1" s="1">
-        <v>9</v>
+        <f>IF(current_round=4,5,9)</f>
+        <v>5</v>
       </c>
       <c r="M1" s="1"/>
     </row>
@@ -2113,24 +2142,24 @@
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="4">
-        <f>SUM(VLOOKUP($B4,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($C4,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($D4,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($E4,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($F4,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($G4,'Raw Data'!$B$2:$R$157,I$1,0))-(par_total*6)</f>
+        <f>SUM(VLOOKUP($B4,'Raw Data'!$B$2:$M$157,I$1,0),VLOOKUP($C4,'Raw Data'!$B$2:$M$157,I$1,0),VLOOKUP($D4,'Raw Data'!$B$2:$M$157,I$1,0),VLOOKUP($E4,'Raw Data'!$B$2:$M$157,I$1,0),VLOOKUP($F4,'Raw Data'!$B$2:$M$157,I$1,0),VLOOKUP($G4,'Raw Data'!$B$2:$M$157,I$1,0))-IF(AND((I$1-current_round)&lt;5,I$1&lt;&gt;5),(6*par_total),0)</f>
         <v>-13</v>
       </c>
       <c r="J4" s="4">
-        <f>SUM(VLOOKUP($B4,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($C4,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($D4,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($E4,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($F4,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($G4,'Raw Data'!$B$2:$R$157,J$1,0))-(par_total*6)</f>
+        <f>SUM(VLOOKUP($B4,'Raw Data'!$B$2:$M$157,J$1,0),VLOOKUP($C4,'Raw Data'!$B$2:$M$157,J$1,0),VLOOKUP($D4,'Raw Data'!$B$2:$M$157,J$1,0),VLOOKUP($E4,'Raw Data'!$B$2:$M$157,J$1,0),VLOOKUP($F4,'Raw Data'!$B$2:$M$157,J$1,0),VLOOKUP($G4,'Raw Data'!$B$2:$M$157,J$1,0))-IF(AND((J$1-current_round)&lt;5,J$1&lt;&gt;5),(6*par_total),0)</f>
         <v>-12</v>
       </c>
       <c r="K4" s="4">
-        <f>SUM(VLOOKUP($B4,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($C4,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($D4,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($E4,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($F4,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($G4,'Raw Data'!$B$2:$R$157,K$1,0))-(par_total*6)</f>
+        <f>SUM(VLOOKUP($B4,'Raw Data'!$B$2:$M$157,K$1,0),VLOOKUP($C4,'Raw Data'!$B$2:$M$157,K$1,0),VLOOKUP($D4,'Raw Data'!$B$2:$M$157,K$1,0),VLOOKUP($E4,'Raw Data'!$B$2:$M$157,K$1,0),VLOOKUP($F4,'Raw Data'!$B$2:$M$157,K$1,0),VLOOKUP($G4,'Raw Data'!$B$2:$M$157,K$1,0))-IF(AND((K$1-current_round)&lt;5,K$1&lt;&gt;5),(6*par_total),0)</f>
         <v>-11</v>
       </c>
       <c r="L4" s="4">
-        <f>SUM(VLOOKUP($B4,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($C4,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($D4,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($E4,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($F4,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($G4,'Raw Data'!$B$2:$R$157,L$1,0))-(par_total*6)</f>
-        <v>-235</v>
+        <f>SUM(VLOOKUP($B4,'Raw Data'!$B$2:$M$157,L$1,0),VLOOKUP($C4,'Raw Data'!$B$2:$M$157,L$1,0),VLOOKUP($D4,'Raw Data'!$B$2:$M$157,L$1,0),VLOOKUP($E4,'Raw Data'!$B$2:$M$157,L$1,0),VLOOKUP($F4,'Raw Data'!$B$2:$M$157,L$1,0),VLOOKUP($G4,'Raw Data'!$B$2:$M$157,L$1,0))-IF(AND((L$1-current_round)&lt;5,L$1&lt;&gt;5),(6*par_total),0)</f>
+        <v>-19</v>
       </c>
       <c r="M4" s="4">
         <f t="shared" ref="M4:M6" si="0">+SUM(I4:L4)</f>
-        <v>-271</v>
+        <v>-55</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2157,24 +2186,24 @@
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="4">
-        <f>SUM(VLOOKUP($B5,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($C5,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($D5,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($E5,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($F5,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($G5,'Raw Data'!$B$2:$R$157,I$1,0))-(par_total*6)</f>
+        <f>SUM(VLOOKUP($B5,'Raw Data'!$B$2:$M$157,I$1,0),VLOOKUP($C5,'Raw Data'!$B$2:$M$157,I$1,0),VLOOKUP($D5,'Raw Data'!$B$2:$M$157,I$1,0),VLOOKUP($E5,'Raw Data'!$B$2:$M$157,I$1,0),VLOOKUP($F5,'Raw Data'!$B$2:$M$157,I$1,0),VLOOKUP($G5,'Raw Data'!$B$2:$M$157,I$1,0))-IF(AND((I$1-current_round)&lt;5,I$1&lt;&gt;5),(6*par_total),0)</f>
         <v>0</v>
       </c>
       <c r="J5" s="4">
-        <f>SUM(VLOOKUP($B5,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($C5,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($D5,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($E5,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($F5,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($G5,'Raw Data'!$B$2:$R$157,J$1,0))-(par_total*6)</f>
+        <f>SUM(VLOOKUP($B5,'Raw Data'!$B$2:$M$157,J$1,0),VLOOKUP($C5,'Raw Data'!$B$2:$M$157,J$1,0),VLOOKUP($D5,'Raw Data'!$B$2:$M$157,J$1,0),VLOOKUP($E5,'Raw Data'!$B$2:$M$157,J$1,0),VLOOKUP($F5,'Raw Data'!$B$2:$M$157,J$1,0),VLOOKUP($G5,'Raw Data'!$B$2:$M$157,J$1,0))-IF(AND((J$1-current_round)&lt;5,J$1&lt;&gt;5),(6*par_total),0)</f>
         <v>-6</v>
       </c>
       <c r="K5" s="4">
-        <f>SUM(VLOOKUP($B5,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($C5,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($D5,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($E5,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($F5,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($G5,'Raw Data'!$B$2:$R$157,K$1,0))-(par_total*6)</f>
+        <f>SUM(VLOOKUP($B5,'Raw Data'!$B$2:$M$157,K$1,0),VLOOKUP($C5,'Raw Data'!$B$2:$M$157,K$1,0),VLOOKUP($D5,'Raw Data'!$B$2:$M$157,K$1,0),VLOOKUP($E5,'Raw Data'!$B$2:$M$157,K$1,0),VLOOKUP($F5,'Raw Data'!$B$2:$M$157,K$1,0),VLOOKUP($G5,'Raw Data'!$B$2:$M$157,K$1,0))-IF(AND((K$1-current_round)&lt;5,K$1&lt;&gt;5),(6*par_total),0)</f>
         <v>-210</v>
       </c>
       <c r="L5" s="4">
-        <f>SUM(VLOOKUP($B5,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($C5,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($D5,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($E5,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($F5,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($G5,'Raw Data'!$B$2:$R$157,L$1,0))-(par_total*6)</f>
-        <v>-432</v>
+        <f>SUM(VLOOKUP($B5,'Raw Data'!$B$2:$M$157,L$1,0),VLOOKUP($C5,'Raw Data'!$B$2:$M$157,L$1,0),VLOOKUP($D5,'Raw Data'!$B$2:$M$157,L$1,0),VLOOKUP($E5,'Raw Data'!$B$2:$M$157,L$1,0),VLOOKUP($F5,'Raw Data'!$B$2:$M$157,L$1,0),VLOOKUP($G5,'Raw Data'!$B$2:$M$157,L$1,0))-IF(AND((L$1-current_round)&lt;5,L$1&lt;&gt;5),(6*par_total),0)</f>
+        <v>0</v>
       </c>
       <c r="M5" s="4">
         <f t="shared" si="0"/>
-        <v>-648</v>
+        <v>-216</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2201,24 +2230,24 @@
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="4">
-        <f>SUM(VLOOKUP($B6,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($C6,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($D6,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($E6,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($F6,'Raw Data'!$B$2:$R$157,I$1,0),VLOOKUP($G6,'Raw Data'!$B$2:$R$157,I$1,0))-(par_total*6)</f>
+        <f>SUM(VLOOKUP($B6,'Raw Data'!$B$2:$M$157,I$1,0),VLOOKUP($C6,'Raw Data'!$B$2:$M$157,I$1,0),VLOOKUP($D6,'Raw Data'!$B$2:$M$157,I$1,0),VLOOKUP($E6,'Raw Data'!$B$2:$M$157,I$1,0),VLOOKUP($F6,'Raw Data'!$B$2:$M$157,I$1,0),VLOOKUP($G6,'Raw Data'!$B$2:$M$157,I$1,0))-IF(AND((I$1-current_round)&lt;5,I$1&lt;&gt;5),(6*par_total),0)</f>
         <v>-28</v>
       </c>
       <c r="J6" s="4">
-        <f>SUM(VLOOKUP($B6,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($C6,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($D6,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($E6,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($F6,'Raw Data'!$B$2:$R$157,J$1,0),VLOOKUP($G6,'Raw Data'!$B$2:$R$157,J$1,0))-(par_total*6)</f>
+        <f>SUM(VLOOKUP($B6,'Raw Data'!$B$2:$M$157,J$1,0),VLOOKUP($C6,'Raw Data'!$B$2:$M$157,J$1,0),VLOOKUP($D6,'Raw Data'!$B$2:$M$157,J$1,0),VLOOKUP($E6,'Raw Data'!$B$2:$M$157,J$1,0),VLOOKUP($F6,'Raw Data'!$B$2:$M$157,J$1,0),VLOOKUP($G6,'Raw Data'!$B$2:$M$157,J$1,0))-IF(AND((J$1-current_round)&lt;5,J$1&lt;&gt;5),(6*par_total),0)</f>
         <v>-167</v>
       </c>
       <c r="K6" s="4">
-        <f>SUM(VLOOKUP($B6,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($C6,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($D6,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($E6,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($F6,'Raw Data'!$B$2:$R$157,K$1,0),VLOOKUP($G6,'Raw Data'!$B$2:$R$157,K$1,0))-(par_total*6)</f>
+        <f>SUM(VLOOKUP($B6,'Raw Data'!$B$2:$M$157,K$1,0),VLOOKUP($C6,'Raw Data'!$B$2:$M$157,K$1,0),VLOOKUP($D6,'Raw Data'!$B$2:$M$157,K$1,0),VLOOKUP($E6,'Raw Data'!$B$2:$M$157,K$1,0),VLOOKUP($F6,'Raw Data'!$B$2:$M$157,K$1,0),VLOOKUP($G6,'Raw Data'!$B$2:$M$157,K$1,0))-IF(AND((K$1-current_round)&lt;5,K$1&lt;&gt;5),(6*par_total),0)</f>
         <v>-432</v>
       </c>
       <c r="L6" s="4">
-        <f>SUM(VLOOKUP($B6,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($C6,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($D6,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($E6,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($F6,'Raw Data'!$B$2:$R$157,L$1,0),VLOOKUP($G6,'Raw Data'!$B$2:$R$157,L$1,0))-(par_total*6)</f>
-        <v>-432</v>
+        <f>SUM(VLOOKUP($B6,'Raw Data'!$B$2:$M$157,L$1,0),VLOOKUP($C6,'Raw Data'!$B$2:$M$157,L$1,0),VLOOKUP($D6,'Raw Data'!$B$2:$M$157,L$1,0),VLOOKUP($E6,'Raw Data'!$B$2:$M$157,L$1,0),VLOOKUP($F6,'Raw Data'!$B$2:$M$157,L$1,0),VLOOKUP($G6,'Raw Data'!$B$2:$M$157,L$1,0))-IF(AND((L$1-current_round)&lt;5,L$1&lt;&gt;5),(6*par_total),0)</f>
+        <v>0</v>
       </c>
       <c r="M6" s="4">
         <f t="shared" si="0"/>
-        <v>-1059</v>
+        <v>-627</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3686,7 +3715,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12176,7 +12205,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12694,11 +12723,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12834,6 +12863,14 @@
         <v>78</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="7">
+        <v>43567.381585648152</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>